<commit_message>
Pruebas con agregar equipo
</commit_message>
<xml_diff>
--- a/Calendario.xlsx
+++ b/Calendario.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rob_a\OneDrive\Documents\NetBeansProjects\LigaAmistad\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="150" yWindow="570" windowWidth="18855" windowHeight="13230"/>
   </bookViews>
@@ -310,7 +315,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -409,6 +414,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -455,7 +468,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -487,9 +500,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -521,6 +535,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -696,7 +711,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">

</xml_diff>

<commit_message>
Muestra la fecha en la tabla, y limpieza de código
</commit_message>
<xml_diff>
--- a/Calendario.xlsx
+++ b/Calendario.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rob_a\OneDrive\Documents\NetBeansProjects\LigaAmistad\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="150" yWindow="570" windowWidth="18855" windowHeight="13230"/>
   </bookViews>
@@ -282,9 +277,6 @@
     <t>Atco. Junior F7</t>
   </si>
   <si>
-    <t>Tratagua's Team</t>
-  </si>
-  <si>
     <t>Valleseco F7 (Retirado)</t>
   </si>
   <si>
@@ -311,11 +303,14 @@
   <si>
     <t>Atl. Platense Fincoman F7</t>
   </si>
+  <si>
+    <t>Trataguas Team</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -468,7 +463,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -500,10 +495,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -535,7 +529,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -711,11 +704,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H1103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -800,11 +793,11 @@
       <c r="C4" s="5"/>
       <c r="D4" s="4"/>
       <c r="E4" s="3" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H4" s="2"/>
     </row>
@@ -818,11 +811,11 @@
       <c r="C5" s="5"/>
       <c r="D5" s="4"/>
       <c r="E5" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H5" s="2"/>
     </row>
@@ -836,11 +829,11 @@
       <c r="C6" s="5"/>
       <c r="D6" s="4"/>
       <c r="E6" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H6" s="2"/>
     </row>
@@ -854,11 +847,11 @@
       <c r="C7" s="5"/>
       <c r="D7" s="4"/>
       <c r="E7" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H7" s="2"/>
     </row>
@@ -872,11 +865,11 @@
       <c r="C8" s="5"/>
       <c r="D8" s="4"/>
       <c r="E8" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H8" s="2"/>
     </row>
@@ -890,11 +883,11 @@
       <c r="C9" s="5"/>
       <c r="D9" s="4"/>
       <c r="E9" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="1" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="H9" s="2"/>
     </row>
@@ -908,11 +901,11 @@
       <c r="C10" s="5"/>
       <c r="D10" s="4"/>
       <c r="E10" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H10" s="2"/>
     </row>
@@ -926,7 +919,7 @@
       <c r="C11" s="5"/>
       <c r="D11" s="4"/>
       <c r="E11" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="1" t="s">
@@ -944,11 +937,11 @@
       <c r="C12" s="5"/>
       <c r="D12" s="4"/>
       <c r="E12" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H12" s="2"/>
     </row>
@@ -962,11 +955,11 @@
       <c r="C13" s="5"/>
       <c r="D13" s="4"/>
       <c r="E13" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H13" s="2"/>
     </row>
@@ -984,7 +977,7 @@
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H14" s="2"/>
     </row>
@@ -1020,7 +1013,7 @@
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H16" s="2"/>
     </row>
@@ -1038,7 +1031,7 @@
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H17" s="2"/>
     </row>
@@ -1052,11 +1045,11 @@
       <c r="C18" s="5"/>
       <c r="D18" s="4"/>
       <c r="E18" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H18" s="2"/>
     </row>
@@ -1070,11 +1063,11 @@
       <c r="C19" s="5"/>
       <c r="D19" s="4"/>
       <c r="E19" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H19" s="2"/>
     </row>
@@ -1088,11 +1081,11 @@
       <c r="C20" s="5"/>
       <c r="D20" s="4"/>
       <c r="E20" s="3" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H20" s="2"/>
     </row>
@@ -1124,11 +1117,11 @@
       <c r="C22" s="5"/>
       <c r="D22" s="4"/>
       <c r="E22" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H22" s="2"/>
     </row>
@@ -1142,7 +1135,7 @@
       <c r="C23" s="5"/>
       <c r="D23" s="4"/>
       <c r="E23" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="1" t="s">
@@ -1160,11 +1153,11 @@
       <c r="C24" s="5"/>
       <c r="D24" s="4"/>
       <c r="E24" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H24" s="2"/>
     </row>
@@ -1178,11 +1171,11 @@
       <c r="C25" s="5"/>
       <c r="D25" s="4"/>
       <c r="E25" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="1" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="H25" s="2"/>
     </row>
@@ -1196,11 +1189,11 @@
       <c r="C26" s="5"/>
       <c r="D26" s="4"/>
       <c r="E26" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H26" s="2"/>
     </row>
@@ -1214,7 +1207,7 @@
       <c r="C27" s="5"/>
       <c r="D27" s="4"/>
       <c r="E27" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="1" t="s">
@@ -1236,7 +1229,7 @@
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H28" s="2"/>
     </row>
@@ -1250,7 +1243,7 @@
       <c r="C29" s="5"/>
       <c r="D29" s="4"/>
       <c r="E29" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="1" t="s">
@@ -1272,7 +1265,7 @@
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H30" s="2"/>
     </row>
@@ -1290,7 +1283,7 @@
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H31" s="2"/>
     </row>
@@ -1304,11 +1297,11 @@
       <c r="C32" s="5"/>
       <c r="D32" s="4"/>
       <c r="E32" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H32" s="2"/>
     </row>
@@ -1326,7 +1319,7 @@
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H33" s="2"/>
     </row>
@@ -1344,7 +1337,7 @@
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H34" s="2"/>
     </row>
@@ -1358,11 +1351,11 @@
       <c r="C35" s="5"/>
       <c r="D35" s="4"/>
       <c r="E35" s="3" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H35" s="2"/>
     </row>
@@ -1376,11 +1369,11 @@
       <c r="C36" s="5"/>
       <c r="D36" s="4"/>
       <c r="E36" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F36" s="2"/>
       <c r="G36" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H36" s="2"/>
     </row>
@@ -1394,7 +1387,7 @@
       <c r="C37" s="5"/>
       <c r="D37" s="4"/>
       <c r="E37" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F37" s="2"/>
       <c r="G37" s="1" t="s">
@@ -1412,11 +1405,11 @@
       <c r="C38" s="5"/>
       <c r="D38" s="4"/>
       <c r="E38" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F38" s="2"/>
       <c r="G38" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H38" s="2"/>
     </row>
@@ -1430,11 +1423,11 @@
       <c r="C39" s="5"/>
       <c r="D39" s="4"/>
       <c r="E39" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F39" s="2"/>
       <c r="G39" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H39" s="2"/>
     </row>
@@ -1448,7 +1441,7 @@
       <c r="C40" s="5"/>
       <c r="D40" s="4"/>
       <c r="E40" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F40" s="2"/>
       <c r="G40" s="1" t="s">
@@ -1466,7 +1459,7 @@
       <c r="C41" s="5"/>
       <c r="D41" s="4"/>
       <c r="E41" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F41" s="2"/>
       <c r="G41" s="1" t="s">
@@ -1484,11 +1477,11 @@
       <c r="C42" s="5"/>
       <c r="D42" s="4"/>
       <c r="E42" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F42" s="2"/>
       <c r="G42" s="1" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="H42" s="2"/>
     </row>
@@ -1502,7 +1495,7 @@
       <c r="C43" s="5"/>
       <c r="D43" s="4"/>
       <c r="E43" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F43" s="2"/>
       <c r="G43" s="1" t="s">
@@ -1520,11 +1513,11 @@
       <c r="C44" s="5"/>
       <c r="D44" s="4"/>
       <c r="E44" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F44" s="2"/>
       <c r="G44" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H44" s="2"/>
     </row>
@@ -1538,11 +1531,11 @@
       <c r="C45" s="5"/>
       <c r="D45" s="4"/>
       <c r="E45" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F45" s="2"/>
       <c r="G45" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H45" s="2"/>
     </row>
@@ -1560,7 +1553,7 @@
       </c>
       <c r="F46" s="2"/>
       <c r="G46" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H46" s="2"/>
     </row>
@@ -1574,11 +1567,11 @@
       <c r="C47" s="5"/>
       <c r="D47" s="4"/>
       <c r="E47" s="3" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="F47" s="2"/>
       <c r="G47" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H47" s="2"/>
     </row>
@@ -1596,7 +1589,7 @@
       </c>
       <c r="F48" s="2"/>
       <c r="G48" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H48" s="2"/>
     </row>
@@ -1614,7 +1607,7 @@
       </c>
       <c r="F49" s="2"/>
       <c r="G49" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H49" s="2"/>
     </row>
@@ -1632,7 +1625,7 @@
       </c>
       <c r="F50" s="2"/>
       <c r="G50" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H50" s="2"/>
     </row>
@@ -1646,7 +1639,7 @@
       <c r="C51" s="5"/>
       <c r="D51" s="4"/>
       <c r="E51" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F51" s="2"/>
       <c r="G51" s="1" t="s">
@@ -1664,11 +1657,11 @@
       <c r="C52" s="5"/>
       <c r="D52" s="4"/>
       <c r="E52" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F52" s="2"/>
       <c r="G52" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H52" s="2"/>
     </row>
@@ -1682,7 +1675,7 @@
       <c r="C53" s="5"/>
       <c r="D53" s="4"/>
       <c r="E53" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F53" s="2"/>
       <c r="G53" s="1" t="s">
@@ -1700,7 +1693,7 @@
       <c r="C54" s="5"/>
       <c r="D54" s="4"/>
       <c r="E54" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F54" s="2"/>
       <c r="G54" s="1" t="s">
@@ -1718,11 +1711,11 @@
       <c r="C55" s="5"/>
       <c r="D55" s="4"/>
       <c r="E55" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F55" s="2"/>
       <c r="G55" s="1" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="H55" s="2"/>
     </row>
@@ -1736,11 +1729,11 @@
       <c r="C56" s="5"/>
       <c r="D56" s="4"/>
       <c r="E56" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F56" s="2"/>
       <c r="G56" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H56" s="2"/>
     </row>
@@ -1754,7 +1747,7 @@
       <c r="C57" s="5"/>
       <c r="D57" s="4"/>
       <c r="E57" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F57" s="2"/>
       <c r="G57" s="1" t="s">
@@ -1776,7 +1769,7 @@
       </c>
       <c r="F58" s="2"/>
       <c r="G58" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H58" s="2"/>
     </row>
@@ -1790,11 +1783,11 @@
       <c r="C59" s="5"/>
       <c r="D59" s="4"/>
       <c r="E59" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F59" s="2"/>
       <c r="G59" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H59" s="2"/>
     </row>
@@ -1808,11 +1801,11 @@
       <c r="C60" s="5"/>
       <c r="D60" s="4"/>
       <c r="E60" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F60" s="2"/>
       <c r="G60" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H60" s="2"/>
     </row>
@@ -1830,7 +1823,7 @@
       </c>
       <c r="F61" s="2"/>
       <c r="G61" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H61" s="2"/>
     </row>
@@ -1848,7 +1841,7 @@
       </c>
       <c r="F62" s="2"/>
       <c r="G62" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H62" s="2"/>
     </row>
@@ -1862,11 +1855,11 @@
       <c r="C63" s="5"/>
       <c r="D63" s="4"/>
       <c r="E63" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F63" s="2"/>
       <c r="G63" s="1" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="H63" s="2"/>
     </row>
@@ -1884,7 +1877,7 @@
       </c>
       <c r="F64" s="2"/>
       <c r="G64" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H64" s="2"/>
     </row>
@@ -1898,7 +1891,7 @@
       <c r="C65" s="5"/>
       <c r="D65" s="4"/>
       <c r="E65" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F65" s="2"/>
       <c r="G65" s="1" t="s">
@@ -1916,11 +1909,11 @@
       <c r="C66" s="5"/>
       <c r="D66" s="4"/>
       <c r="E66" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F66" s="2"/>
       <c r="G66" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H66" s="2"/>
     </row>
@@ -1934,11 +1927,11 @@
       <c r="C67" s="5"/>
       <c r="D67" s="4"/>
       <c r="E67" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F67" s="2"/>
       <c r="G67" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H67" s="2"/>
     </row>
@@ -1952,7 +1945,7 @@
       <c r="C68" s="5"/>
       <c r="D68" s="4"/>
       <c r="E68" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F68" s="2"/>
       <c r="G68" s="1" t="s">
@@ -1970,7 +1963,7 @@
       <c r="C69" s="5"/>
       <c r="D69" s="4"/>
       <c r="E69" s="3" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="F69" s="2"/>
       <c r="G69" s="1" t="s">
@@ -1988,7 +1981,7 @@
       <c r="C70" s="5"/>
       <c r="D70" s="4"/>
       <c r="E70" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F70" s="2"/>
       <c r="G70" s="1" t="s">
@@ -2006,11 +1999,11 @@
       <c r="C71" s="5"/>
       <c r="D71" s="4"/>
       <c r="E71" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F71" s="2"/>
       <c r="G71" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H71" s="2"/>
     </row>
@@ -2024,11 +2017,11 @@
       <c r="C72" s="5"/>
       <c r="D72" s="4"/>
       <c r="E72" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F72" s="2"/>
       <c r="G72" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H72" s="2"/>
     </row>
@@ -2046,7 +2039,7 @@
       </c>
       <c r="F73" s="2"/>
       <c r="G73" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H73" s="2"/>
     </row>
@@ -2060,11 +2053,11 @@
       <c r="C74" s="5"/>
       <c r="D74" s="4"/>
       <c r="E74" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F74" s="2"/>
       <c r="G74" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H74" s="2"/>
     </row>
@@ -2082,7 +2075,7 @@
       </c>
       <c r="F75" s="2"/>
       <c r="G75" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H75" s="2"/>
     </row>
@@ -2100,7 +2093,7 @@
       </c>
       <c r="F76" s="2"/>
       <c r="G76" s="1" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="H76" s="2"/>
     </row>
@@ -2114,7 +2107,7 @@
       <c r="C77" s="5"/>
       <c r="D77" s="4"/>
       <c r="E77" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F77" s="2"/>
       <c r="G77" s="1" t="s">
@@ -2132,11 +2125,11 @@
       <c r="C78" s="5"/>
       <c r="D78" s="4"/>
       <c r="E78" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F78" s="2"/>
       <c r="G78" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H78" s="2"/>
     </row>
@@ -2150,11 +2143,11 @@
       <c r="C79" s="2"/>
       <c r="D79" s="4"/>
       <c r="E79" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F79" s="2"/>
       <c r="G79" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H79" s="2"/>
     </row>
@@ -2168,11 +2161,11 @@
       <c r="C80" s="5"/>
       <c r="D80" s="4"/>
       <c r="E80" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F80" s="2"/>
       <c r="G80" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H80" s="2"/>
     </row>
@@ -2186,7 +2179,7 @@
       <c r="C81" s="5"/>
       <c r="D81" s="4"/>
       <c r="E81" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F81" s="2"/>
       <c r="G81" s="1" t="s">
@@ -2204,11 +2197,11 @@
       <c r="C82" s="5"/>
       <c r="D82" s="4"/>
       <c r="E82" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F82" s="2"/>
       <c r="G82" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H82" s="2"/>
     </row>
@@ -2222,11 +2215,11 @@
       <c r="C83" s="5"/>
       <c r="D83" s="4"/>
       <c r="E83" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F83" s="2"/>
       <c r="G83" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H83" s="2"/>
     </row>
@@ -2258,7 +2251,7 @@
       <c r="C85" s="5"/>
       <c r="D85" s="4"/>
       <c r="E85" s="3" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="F85" s="2"/>
       <c r="G85" s="1" t="s">
@@ -2276,11 +2269,11 @@
       <c r="C86" s="2"/>
       <c r="D86" s="4"/>
       <c r="E86" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F86" s="2"/>
       <c r="G86" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H86" s="2"/>
     </row>
@@ -2298,7 +2291,7 @@
       </c>
       <c r="F87" s="2"/>
       <c r="G87" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H87" s="2"/>
     </row>
@@ -2312,11 +2305,11 @@
       <c r="C88" s="5"/>
       <c r="D88" s="4"/>
       <c r="E88" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F88" s="2"/>
       <c r="G88" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H88" s="2"/>
     </row>
@@ -2330,11 +2323,11 @@
       <c r="C89" s="5"/>
       <c r="D89" s="4"/>
       <c r="E89" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F89" s="2"/>
       <c r="G89" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H89" s="2"/>
     </row>
@@ -2348,11 +2341,11 @@
       <c r="C90" s="5"/>
       <c r="D90" s="4"/>
       <c r="E90" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F90" s="2"/>
       <c r="G90" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H90" s="2"/>
     </row>
@@ -2388,7 +2381,7 @@
       </c>
       <c r="F92" s="2"/>
       <c r="G92" s="1" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="H92" s="2"/>
     </row>
@@ -2402,11 +2395,11 @@
       <c r="C93" s="2"/>
       <c r="D93" s="4"/>
       <c r="E93" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F93" s="2"/>
       <c r="G93" s="1" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="H93" s="2"/>
     </row>
@@ -2420,11 +2413,11 @@
       <c r="C94" s="5"/>
       <c r="D94" s="4"/>
       <c r="E94" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F94" s="2"/>
       <c r="G94" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H94" s="2"/>
     </row>
@@ -2438,11 +2431,11 @@
       <c r="C95" s="5"/>
       <c r="D95" s="4"/>
       <c r="E95" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F95" s="2"/>
       <c r="G95" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H95" s="2"/>
     </row>
@@ -2474,11 +2467,11 @@
       <c r="C97" s="5"/>
       <c r="D97" s="4"/>
       <c r="E97" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F97" s="2"/>
       <c r="G97" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H97" s="2"/>
     </row>
@@ -2510,11 +2503,11 @@
       <c r="C99" s="5"/>
       <c r="D99" s="4"/>
       <c r="E99" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F99" s="2"/>
       <c r="G99" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H99" s="2"/>
     </row>
@@ -2532,7 +2525,7 @@
       </c>
       <c r="F100" s="2"/>
       <c r="G100" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H100" s="2"/>
     </row>
@@ -2546,11 +2539,11 @@
       <c r="C101" s="5"/>
       <c r="D101" s="4"/>
       <c r="E101" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F101" s="2"/>
       <c r="G101" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H101" s="2"/>
     </row>
@@ -2582,11 +2575,11 @@
       <c r="C103" s="5"/>
       <c r="D103" s="4"/>
       <c r="E103" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F103" s="2"/>
       <c r="G103" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H103" s="2"/>
     </row>
@@ -2600,11 +2593,11 @@
       <c r="C104" s="5"/>
       <c r="D104" s="4"/>
       <c r="E104" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F104" s="2"/>
       <c r="G104" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H104" s="2"/>
     </row>
@@ -2618,11 +2611,11 @@
       <c r="C105" s="5"/>
       <c r="D105" s="4"/>
       <c r="E105" s="3" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="F105" s="2"/>
       <c r="G105" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H105" s="2"/>
     </row>
@@ -2636,7 +2629,7 @@
       <c r="C106" s="5"/>
       <c r="D106" s="4"/>
       <c r="E106" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F106" s="2"/>
       <c r="G106" s="1" t="s">
@@ -2654,7 +2647,7 @@
       <c r="C107" s="2"/>
       <c r="D107" s="4"/>
       <c r="E107" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F107" s="2"/>
       <c r="G107" s="1" t="s">
@@ -2672,11 +2665,11 @@
       <c r="C108" s="5"/>
       <c r="D108" s="4"/>
       <c r="E108" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F108" s="2"/>
       <c r="G108" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H108" s="2"/>
     </row>
@@ -2690,11 +2683,11 @@
       <c r="C109" s="5"/>
       <c r="D109" s="4"/>
       <c r="E109" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F109" s="2"/>
       <c r="G109" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H109" s="2"/>
     </row>
@@ -2708,11 +2701,11 @@
       <c r="C110" s="5"/>
       <c r="D110" s="4"/>
       <c r="E110" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F110" s="2"/>
       <c r="G110" s="1" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="H110" s="2"/>
     </row>
@@ -2726,11 +2719,11 @@
       <c r="C111" s="5"/>
       <c r="D111" s="4"/>
       <c r="E111" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F111" s="2"/>
       <c r="G111" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H111" s="2"/>
     </row>
@@ -2762,7 +2755,7 @@
       <c r="C113" s="5"/>
       <c r="D113" s="4"/>
       <c r="E113" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F113" s="2"/>
       <c r="G113" s="1" t="s">
@@ -2784,7 +2777,7 @@
       </c>
       <c r="F114" s="2"/>
       <c r="G114" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H114" s="2"/>
     </row>
@@ -2798,11 +2791,11 @@
       <c r="C115" s="5"/>
       <c r="D115" s="4"/>
       <c r="E115" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F115" s="2"/>
       <c r="G115" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H115" s="2"/>
     </row>
@@ -2816,11 +2809,11 @@
       <c r="C116" s="5"/>
       <c r="D116" s="4"/>
       <c r="E116" s="3" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="F116" s="2"/>
       <c r="G116" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H116" s="2"/>
     </row>
@@ -2838,7 +2831,7 @@
       </c>
       <c r="F117" s="2"/>
       <c r="G117" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H117" s="2"/>
     </row>
@@ -2852,11 +2845,11 @@
       <c r="C118" s="5"/>
       <c r="D118" s="4"/>
       <c r="E118" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F118" s="2"/>
       <c r="G118" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H118" s="2"/>
     </row>
@@ -2870,7 +2863,7 @@
       <c r="C119" s="5"/>
       <c r="D119" s="4"/>
       <c r="E119" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F119" s="2"/>
       <c r="G119" s="1" t="s">
@@ -2892,7 +2885,7 @@
       </c>
       <c r="F120" s="2"/>
       <c r="G120" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H120" s="2"/>
     </row>
@@ -2906,7 +2899,7 @@
       <c r="C121" s="2"/>
       <c r="D121" s="4"/>
       <c r="E121" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F121" s="2"/>
       <c r="G121" s="1" t="s">
@@ -2924,11 +2917,11 @@
       <c r="C122" s="5"/>
       <c r="D122" s="4"/>
       <c r="E122" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F122" s="2"/>
       <c r="G122" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H122" s="2"/>
     </row>
@@ -2942,11 +2935,11 @@
       <c r="C123" s="5"/>
       <c r="D123" s="4"/>
       <c r="E123" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F123" s="2"/>
       <c r="G123" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H123" s="2"/>
     </row>
@@ -2960,7 +2953,7 @@
       <c r="C124" s="5"/>
       <c r="D124" s="4"/>
       <c r="E124" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F124" s="2"/>
       <c r="G124" s="1" t="s">
@@ -2978,11 +2971,11 @@
       <c r="C125" s="5"/>
       <c r="D125" s="4"/>
       <c r="E125" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F125" s="2"/>
       <c r="G125" s="1" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="H125" s="2"/>
     </row>
@@ -2996,7 +2989,7 @@
       <c r="C126" s="5"/>
       <c r="D126" s="4"/>
       <c r="E126" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F126" s="2"/>
       <c r="G126" s="1" t="s">
@@ -3014,7 +3007,7 @@
       <c r="C127" s="5"/>
       <c r="D127" s="4"/>
       <c r="E127" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F127" s="2"/>
       <c r="G127" s="1" t="s">
@@ -3032,11 +3025,11 @@
       <c r="C128" s="2"/>
       <c r="D128" s="4"/>
       <c r="E128" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F128" s="2"/>
       <c r="G128" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H128" s="2"/>
     </row>
@@ -3050,11 +3043,11 @@
       <c r="C129" s="5"/>
       <c r="D129" s="4"/>
       <c r="E129" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F129" s="2"/>
       <c r="G129" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H129" s="2"/>
     </row>
@@ -3068,11 +3061,11 @@
       <c r="C130" s="5"/>
       <c r="D130" s="4"/>
       <c r="E130" s="3" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="F130" s="2"/>
       <c r="G130" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H130" s="2"/>
     </row>
@@ -3090,7 +3083,7 @@
       </c>
       <c r="F131" s="2"/>
       <c r="G131" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H131" s="2"/>
     </row>
@@ -3108,7 +3101,7 @@
       </c>
       <c r="F132" s="2"/>
       <c r="G132" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H132" s="2"/>
     </row>
@@ -3126,7 +3119,7 @@
       </c>
       <c r="F133" s="2"/>
       <c r="G133" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H133" s="2"/>
     </row>
@@ -3144,7 +3137,7 @@
       </c>
       <c r="F134" s="2"/>
       <c r="G134" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H134" s="2"/>
     </row>
@@ -3158,11 +3151,11 @@
       <c r="C135" s="2"/>
       <c r="D135" s="4"/>
       <c r="E135" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F135" s="2"/>
       <c r="G135" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H135" s="2"/>
     </row>
@@ -3176,11 +3169,11 @@
       <c r="C136" s="5"/>
       <c r="D136" s="4"/>
       <c r="E136" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F136" s="2"/>
       <c r="G136" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H136" s="2"/>
     </row>
@@ -3194,11 +3187,11 @@
       <c r="C137" s="5"/>
       <c r="D137" s="4"/>
       <c r="E137" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F137" s="2"/>
       <c r="G137" s="1" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="H137" s="2"/>
     </row>
@@ -3212,7 +3205,7 @@
       <c r="C138" s="5"/>
       <c r="D138" s="4"/>
       <c r="E138" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F138" s="2"/>
       <c r="G138" s="1" t="s">
@@ -3230,7 +3223,7 @@
       <c r="C139" s="5"/>
       <c r="D139" s="4"/>
       <c r="E139" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F139" s="2"/>
       <c r="G139" s="1" t="s">
@@ -3248,7 +3241,7 @@
       <c r="C140" s="5"/>
       <c r="D140" s="4"/>
       <c r="E140" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F140" s="2"/>
       <c r="G140" s="1" t="s">
@@ -3266,7 +3259,7 @@
       <c r="C141" s="5"/>
       <c r="D141" s="4"/>
       <c r="E141" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F141" s="2"/>
       <c r="G141" s="1" t="s">
@@ -3284,11 +3277,11 @@
       <c r="C142" s="2"/>
       <c r="D142" s="4"/>
       <c r="E142" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F142" s="2"/>
       <c r="G142" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H142" s="2"/>
     </row>
@@ -3306,7 +3299,7 @@
       </c>
       <c r="F143" s="2"/>
       <c r="G143" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H143" s="2"/>
     </row>
@@ -3324,7 +3317,7 @@
       </c>
       <c r="F144" s="2"/>
       <c r="G144" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H144" s="2"/>
     </row>
@@ -3338,11 +3331,11 @@
       <c r="C145" s="5"/>
       <c r="D145" s="4"/>
       <c r="E145" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F145" s="2"/>
       <c r="G145" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H145" s="2"/>
     </row>
@@ -3360,7 +3353,7 @@
       </c>
       <c r="F146" s="2"/>
       <c r="G146" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H146" s="2"/>
     </row>
@@ -3374,11 +3367,11 @@
       <c r="C147" s="5"/>
       <c r="D147" s="4"/>
       <c r="E147" s="3" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="F147" s="2"/>
       <c r="G147" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H147" s="2"/>
     </row>
@@ -3396,7 +3389,7 @@
       </c>
       <c r="F148" s="2"/>
       <c r="G148" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H148" s="2"/>
     </row>
@@ -3410,11 +3403,11 @@
       <c r="C149" s="2"/>
       <c r="D149" s="4"/>
       <c r="E149" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F149" s="2"/>
       <c r="G149" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H149" s="2"/>
     </row>
@@ -3428,11 +3421,11 @@
       <c r="C150" s="5"/>
       <c r="D150" s="4"/>
       <c r="E150" s="3" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="F150" s="2"/>
       <c r="G150" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H150" s="2"/>
     </row>
@@ -3446,7 +3439,7 @@
       <c r="C151" s="5"/>
       <c r="D151" s="4"/>
       <c r="E151" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F151" s="2"/>
       <c r="G151" s="1" t="s">
@@ -3464,7 +3457,7 @@
       <c r="C152" s="5"/>
       <c r="D152" s="4"/>
       <c r="E152" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F152" s="2"/>
       <c r="G152" s="1" t="s">
@@ -3482,11 +3475,11 @@
       <c r="C153" s="5"/>
       <c r="D153" s="4"/>
       <c r="E153" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F153" s="2"/>
       <c r="G153" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H153" s="2"/>
     </row>
@@ -3500,7 +3493,7 @@
       <c r="C154" s="5"/>
       <c r="D154" s="4"/>
       <c r="E154" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F154" s="2"/>
       <c r="G154" s="1" t="s">
@@ -3518,7 +3511,7 @@
       <c r="C155" s="5"/>
       <c r="D155" s="4"/>
       <c r="E155" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F155" s="2"/>
       <c r="G155" s="1" t="s">
@@ -3536,11 +3529,11 @@
       <c r="C156" s="2"/>
       <c r="D156" s="4"/>
       <c r="E156" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F156" s="2"/>
       <c r="G156" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H156" s="2"/>
     </row>
@@ -3554,11 +3547,11 @@
       <c r="C157" s="5"/>
       <c r="D157" s="4"/>
       <c r="E157" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F157" s="2"/>
       <c r="G157" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H157" s="2"/>
     </row>
@@ -3572,11 +3565,11 @@
       <c r="C158" s="5"/>
       <c r="D158" s="4"/>
       <c r="E158" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F158" s="2"/>
       <c r="G158" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H158" s="2"/>
     </row>
@@ -3594,7 +3587,7 @@
       </c>
       <c r="F159" s="2"/>
       <c r="G159" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H159" s="2"/>
     </row>
@@ -3612,7 +3605,7 @@
       </c>
       <c r="F160" s="2"/>
       <c r="G160" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H160" s="2"/>
     </row>
@@ -3630,7 +3623,7 @@
       </c>
       <c r="F161" s="2"/>
       <c r="G161" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H161" s="2"/>
     </row>
@@ -3648,7 +3641,7 @@
       </c>
       <c r="F162" s="2"/>
       <c r="G162" s="1" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="H162" s="2"/>
     </row>
@@ -3662,11 +3655,11 @@
       <c r="C163" s="2"/>
       <c r="D163" s="4"/>
       <c r="E163" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F163" s="2"/>
       <c r="G163" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H163" s="2"/>
     </row>
@@ -3680,11 +3673,11 @@
       <c r="C164" s="5"/>
       <c r="D164" s="4"/>
       <c r="E164" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F164" s="2"/>
       <c r="G164" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H164" s="2"/>
     </row>
@@ -3698,7 +3691,7 @@
       <c r="C165" s="5"/>
       <c r="D165" s="4"/>
       <c r="E165" s="3" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="F165" s="2"/>
       <c r="G165" s="1" t="s">
@@ -3716,7 +3709,7 @@
       <c r="C166" s="5"/>
       <c r="D166" s="4"/>
       <c r="E166" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F166" s="2"/>
       <c r="G166" s="1" t="s">
@@ -3734,11 +3727,11 @@
       <c r="C167" s="5"/>
       <c r="D167" s="4"/>
       <c r="E167" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F167" s="2"/>
       <c r="G167" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H167" s="2"/>
     </row>
@@ -3752,7 +3745,7 @@
       <c r="C168" s="5"/>
       <c r="D168" s="4"/>
       <c r="E168" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F168" s="2"/>
       <c r="G168" s="1" t="s">
@@ -3774,7 +3767,7 @@
       </c>
       <c r="F169" s="2"/>
       <c r="G169" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H169" s="2"/>
     </row>
@@ -3788,11 +3781,11 @@
       <c r="C170" s="2"/>
       <c r="D170" s="4"/>
       <c r="E170" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F170" s="2"/>
       <c r="G170" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H170" s="2"/>
     </row>
@@ -3806,11 +3799,11 @@
       <c r="C171" s="5"/>
       <c r="D171" s="4"/>
       <c r="E171" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F171" s="2"/>
       <c r="G171" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H171" s="2"/>
     </row>
@@ -3824,11 +3817,11 @@
       <c r="C172" s="5"/>
       <c r="D172" s="4"/>
       <c r="E172" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F172" s="2"/>
       <c r="G172" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H172" s="2"/>
     </row>
@@ -3842,11 +3835,11 @@
       <c r="C173" s="5"/>
       <c r="D173" s="4"/>
       <c r="E173" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F173" s="2"/>
       <c r="G173" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H173" s="2"/>
     </row>
@@ -3882,7 +3875,7 @@
       </c>
       <c r="F175" s="2"/>
       <c r="G175" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H175" s="2"/>
     </row>
@@ -3900,7 +3893,7 @@
       </c>
       <c r="F176" s="2"/>
       <c r="G176" s="1" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="H176" s="2"/>
     </row>
@@ -3914,11 +3907,11 @@
       <c r="C177" s="2"/>
       <c r="D177" s="4"/>
       <c r="E177" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F177" s="2"/>
       <c r="G177" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H177" s="2"/>
     </row>
@@ -3932,7 +3925,7 @@
       <c r="C178" s="2"/>
       <c r="D178" s="4"/>
       <c r="E178" s="3" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="F178" s="2"/>
       <c r="G178" s="1" t="s">
@@ -3950,7 +3943,7 @@
       <c r="C179" s="2"/>
       <c r="D179" s="4"/>
       <c r="E179" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F179" s="2"/>
       <c r="G179" s="1" t="s">
@@ -3986,11 +3979,11 @@
       <c r="C181" s="2"/>
       <c r="D181" s="4"/>
       <c r="E181" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F181" s="2"/>
       <c r="G181" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H181" s="2"/>
     </row>
@@ -4004,11 +3997,11 @@
       <c r="C182" s="2"/>
       <c r="D182" s="4"/>
       <c r="E182" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F182" s="2"/>
       <c r="G182" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H182" s="2"/>
     </row>
@@ -4022,11 +4015,11 @@
       <c r="C183" s="2"/>
       <c r="D183" s="4"/>
       <c r="E183" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F183" s="2"/>
       <c r="G183" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H183" s="2"/>
     </row>

</xml_diff>

<commit_message>
Solucionado error al leer excel
</commit_message>
<xml_diff>
--- a/Calendario.xlsx
+++ b/Calendario.xlsx
@@ -304,7 +304,7 @@
     <t>Atl. Platense Fincoman F7</t>
   </si>
   <si>
-    <t>Trataguas Team</t>
+    <t>Tratagua's Team</t>
   </si>
 </sst>
 </file>
@@ -708,7 +708,7 @@
   <dimension ref="A1:H1103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>

</xml_diff>